<commit_message>
use sockets, so you can telnet in character mode
</commit_message>
<xml_diff>
--- a/Instructions.xlsx
+++ b/Instructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Code/DEVIN/A_8080/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F98AEF03-B39D-A840-846F-A5CAA6FDC0A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CC3FCB-CA97-CC4A-8E2E-29975ACB2EF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" xr2:uid="{353367B8-2C40-2F48-BA34-9B147C977459}"/>
   </bookViews>
@@ -1607,7 +1607,7 @@
   <dimension ref="A1:Q53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P49" sqref="P49:P51"/>
+      <selection activeCell="E12" sqref="E10:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4253,6 +4253,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A16:A18"/>
     <mergeCell ref="A40:A42"/>
     <mergeCell ref="A43:A45"/>
     <mergeCell ref="A46:A48"/>
@@ -4263,12 +4269,6 @@
     <mergeCell ref="A31:A33"/>
     <mergeCell ref="A34:A36"/>
     <mergeCell ref="A37:A39"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="A16:A18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix keyboard stuff, curses borders and titles, VIO resizing, disk commands via device outputs
</commit_message>
<xml_diff>
--- a/Instructions.xlsx
+++ b/Instructions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Code/DEVIN/A_8080/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CC3FCB-CA97-CC4A-8E2E-29975ACB2EF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ABB9C2D-66C7-0349-B92A-5674429AA444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" xr2:uid="{353367B8-2C40-2F48-BA34-9B147C977459}"/>
   </bookViews>
@@ -939,7 +939,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -987,6 +987,12 @@
     <font>
       <b/>
       <sz val="10"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
       <name val="Courier New"/>
       <family val="1"/>
     </font>
@@ -1217,7 +1223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1245,9 +1251,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1257,9 +1260,6 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1281,9 +1281,18 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1606,8 +1615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99D68540-6623-E94B-BB1D-1096F1E0F79F}">
   <dimension ref="A1:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E12" sqref="E10:E12"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M49" sqref="M49:M51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1619,16 +1628,16 @@
     </row>
     <row r="2" spans="1:17" ht="19" thickBot="1">
       <c r="A2" s="2"/>
-      <c r="J2" s="60" t="s">
+      <c r="J2" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="61" t="s">
+      <c r="K2" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="61" t="s">
+      <c r="L2" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="61" t="s">
+      <c r="M2" s="55" t="s">
         <v>4</v>
       </c>
       <c r="N2" s="4" t="s">
@@ -1646,16 +1655,16 @@
     </row>
     <row r="3" spans="1:17" ht="17" thickBot="1">
       <c r="A3" s="3"/>
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="61" t="s">
+      <c r="C3" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="61" t="s">
+      <c r="D3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="61" t="s">
+      <c r="E3" s="55" t="s">
         <v>4</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -1670,16 +1679,16 @@
       <c r="I3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="61" t="s">
+      <c r="J3" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="61" t="s">
+      <c r="K3" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="61" t="s">
+      <c r="L3" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="61" t="s">
+      <c r="M3" s="55" t="s">
         <v>12</v>
       </c>
       <c r="N3" s="4" t="s">
@@ -1696,7 +1705,7 @@
       </c>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="57" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -1749,7 +1758,7 @@
       </c>
     </row>
     <row r="5" spans="1:17">
-      <c r="A5" s="64"/>
+      <c r="A5" s="58"/>
       <c r="B5" s="6" t="s">
         <v>19</v>
       </c>
@@ -1800,7 +1809,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" ht="17" thickBot="1">
-      <c r="A6" s="64"/>
+      <c r="A6" s="58"/>
       <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
@@ -1851,7 +1860,7 @@
       </c>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="58" t="s">
         <v>43</v>
       </c>
       <c r="B7" s="8" t="s">
@@ -1904,7 +1913,7 @@
       </c>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="64"/>
+      <c r="A8" s="58"/>
       <c r="B8" s="6" t="s">
         <v>19</v>
       </c>
@@ -1955,7 +1964,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" ht="17" thickBot="1">
-      <c r="A9" s="64"/>
+      <c r="A9" s="58"/>
       <c r="B9" s="7" t="s">
         <v>20</v>
       </c>
@@ -2006,7 +2015,7 @@
       </c>
     </row>
     <row r="10" spans="1:17">
-      <c r="A10" s="64" t="s">
+      <c r="A10" s="58" t="s">
         <v>58</v>
       </c>
       <c r="B10" s="8" t="s">
@@ -2015,31 +2024,31 @@
       <c r="C10" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="D10" s="57" t="s">
+      <c r="D10" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="E10" s="45" t="s">
+      <c r="E10" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="F10" s="46" t="s">
+      <c r="F10" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="G10" s="46" t="s">
+      <c r="G10" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="H10" s="47" t="s">
+      <c r="H10" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="I10" s="46" t="s">
+      <c r="I10" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="J10" s="48" t="s">
+      <c r="J10" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="K10" s="45" t="s">
+      <c r="K10" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="L10" s="57" t="s">
+      <c r="L10" s="51" t="s">
         <v>69</v>
       </c>
       <c r="M10" s="17" t="s">
@@ -2059,38 +2068,38 @@
       </c>
     </row>
     <row r="11" spans="1:17">
-      <c r="A11" s="64"/>
+      <c r="A11" s="58"/>
       <c r="B11" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="58" t="s">
+      <c r="D11" s="52" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="H11" s="51" t="s">
+      <c r="E11" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="I11" s="50" t="s">
-        <v>19</v>
-      </c>
-      <c r="J11" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="K11" s="49" t="s">
+      <c r="I11" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="L11" s="58" t="s">
+      <c r="L11" s="52" t="s">
         <v>61</v>
       </c>
       <c r="M11" s="15" t="s">
@@ -2110,38 +2119,38 @@
       </c>
     </row>
     <row r="12" spans="1:17" ht="17" thickBot="1">
-      <c r="A12" s="64"/>
+      <c r="A12" s="58"/>
       <c r="B12" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="59" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="53" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="54" t="s">
+      <c r="D12" s="53" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="54" t="s">
+      <c r="G12" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="H12" s="55" t="s">
-        <v>20</v>
-      </c>
-      <c r="I12" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="J12" s="56" t="s">
-        <v>20</v>
-      </c>
-      <c r="K12" s="53" t="s">
+      <c r="H12" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="J12" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="K12" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="L12" s="59" t="s">
+      <c r="L12" s="53" t="s">
         <v>20</v>
       </c>
       <c r="M12" s="16" t="s">
@@ -2161,7 +2170,7 @@
       </c>
     </row>
     <row r="13" spans="1:17">
-      <c r="A13" s="64" t="s">
+      <c r="A13" s="58" t="s">
         <v>75</v>
       </c>
       <c r="B13" s="8" t="s">
@@ -2170,31 +2179,31 @@
       <c r="C13" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="D13" s="47" t="s">
+      <c r="D13" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="E13" s="45" t="s">
+      <c r="E13" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="F13" s="46" t="s">
+      <c r="F13" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="G13" s="46" t="s">
+      <c r="G13" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="H13" s="47" t="s">
+      <c r="H13" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="I13" s="46" t="s">
+      <c r="I13" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="J13" s="48" t="s">
+      <c r="J13" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="K13" s="45" t="s">
+      <c r="K13" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="L13" s="47" t="s">
+      <c r="L13" s="41" t="s">
         <v>86</v>
       </c>
       <c r="M13" s="17" t="s">
@@ -2214,38 +2223,38 @@
       </c>
     </row>
     <row r="14" spans="1:17">
-      <c r="A14" s="64"/>
+      <c r="A14" s="58"/>
       <c r="B14" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="51" t="s">
+      <c r="D14" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="E14" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" s="50" t="s">
+      <c r="E14" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="G14" s="50" t="s">
+      <c r="G14" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="H14" s="51" t="s">
+      <c r="H14" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="I14" s="50" t="s">
-        <v>19</v>
-      </c>
-      <c r="J14" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="K14" s="49" t="s">
+      <c r="I14" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="L14" s="51" t="s">
+      <c r="L14" s="45" t="s">
         <v>78</v>
       </c>
       <c r="M14" s="15" t="s">
@@ -2265,38 +2274,38 @@
       </c>
     </row>
     <row r="15" spans="1:17" ht="17" thickBot="1">
-      <c r="A15" s="64"/>
+      <c r="A15" s="58"/>
       <c r="B15" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="55" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="53" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="54" t="s">
+      <c r="D15" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="54" t="s">
+      <c r="G15" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="H15" s="55" t="s">
-        <v>20</v>
-      </c>
-      <c r="I15" s="54" t="s">
+      <c r="H15" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="I15" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="J15" s="56" t="s">
-        <v>20</v>
-      </c>
-      <c r="K15" s="53" t="s">
+      <c r="J15" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="K15" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="L15" s="55" t="s">
+      <c r="L15" s="49" t="s">
         <v>20</v>
       </c>
       <c r="M15" s="16" t="s">
@@ -2316,7 +2325,7 @@
       </c>
     </row>
     <row r="16" spans="1:17">
-      <c r="A16" s="62" t="s">
+      <c r="A16" s="56" t="s">
         <v>92</v>
       </c>
       <c r="B16" s="18" t="s">
@@ -2369,7 +2378,7 @@
       </c>
     </row>
     <row r="17" spans="1:17">
-      <c r="A17" s="62"/>
+      <c r="A17" s="56"/>
       <c r="B17" s="20" t="s">
         <v>26</v>
       </c>
@@ -2420,7 +2429,7 @@
       </c>
     </row>
     <row r="18" spans="1:17" ht="17" thickBot="1">
-      <c r="A18" s="62"/>
+      <c r="A18" s="56"/>
       <c r="B18" s="22" t="s">
         <v>20</v>
       </c>
@@ -2471,7 +2480,7 @@
       </c>
     </row>
     <row r="19" spans="1:17">
-      <c r="A19" s="62" t="s">
+      <c r="A19" s="56" t="s">
         <v>109</v>
       </c>
       <c r="B19" s="18" t="s">
@@ -2524,7 +2533,7 @@
       </c>
     </row>
     <row r="20" spans="1:17">
-      <c r="A20" s="62"/>
+      <c r="A20" s="56"/>
       <c r="B20" s="20" t="s">
         <v>26</v>
       </c>
@@ -2575,7 +2584,7 @@
       </c>
     </row>
     <row r="21" spans="1:17" ht="17" thickBot="1">
-      <c r="A21" s="62"/>
+      <c r="A21" s="56"/>
       <c r="B21" s="22" t="s">
         <v>20</v>
       </c>
@@ -2626,7 +2635,7 @@
       </c>
     </row>
     <row r="22" spans="1:17">
-      <c r="A22" s="62" t="s">
+      <c r="A22" s="56" t="s">
         <v>126</v>
       </c>
       <c r="B22" s="18" t="s">
@@ -2679,7 +2688,7 @@
       </c>
     </row>
     <row r="23" spans="1:17">
-      <c r="A23" s="62"/>
+      <c r="A23" s="56"/>
       <c r="B23" s="20" t="s">
         <v>26</v>
       </c>
@@ -2730,7 +2739,7 @@
       </c>
     </row>
     <row r="24" spans="1:17" ht="17" thickBot="1">
-      <c r="A24" s="62"/>
+      <c r="A24" s="56"/>
       <c r="B24" s="22" t="s">
         <v>20</v>
       </c>
@@ -2781,7 +2790,7 @@
       </c>
     </row>
     <row r="25" spans="1:17">
-      <c r="A25" s="62" t="s">
+      <c r="A25" s="56" t="s">
         <v>143</v>
       </c>
       <c r="B25" s="18" t="s">
@@ -2834,7 +2843,7 @@
       </c>
     </row>
     <row r="26" spans="1:17">
-      <c r="A26" s="62"/>
+      <c r="A26" s="56"/>
       <c r="B26" s="20" t="s">
         <v>24</v>
       </c>
@@ -2885,7 +2894,7 @@
       </c>
     </row>
     <row r="27" spans="1:17" ht="17" thickBot="1">
-      <c r="A27" s="62"/>
+      <c r="A27" s="56"/>
       <c r="B27" s="22" t="s">
         <v>20</v>
       </c>
@@ -2936,10 +2945,10 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="A28" s="64" t="s">
+      <c r="A28" s="58" t="s">
         <v>160</v>
       </c>
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="27" t="s">
         <v>161</v>
       </c>
       <c r="C28" s="26" t="s">
@@ -2989,8 +2998,8 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="A29" s="64"/>
-      <c r="B29" s="31" t="s">
+      <c r="A29" s="58"/>
+      <c r="B29" s="28" t="s">
         <v>19</v>
       </c>
       <c r="C29" s="24" t="s">
@@ -3040,8 +3049,8 @@
       </c>
     </row>
     <row r="30" spans="1:17" ht="17" thickBot="1">
-      <c r="A30" s="64"/>
-      <c r="B30" s="32" t="s">
+      <c r="A30" s="58"/>
+      <c r="B30" s="29" t="s">
         <v>67</v>
       </c>
       <c r="C30" s="25" t="s">
@@ -3091,10 +3100,10 @@
       </c>
     </row>
     <row r="31" spans="1:17">
-      <c r="A31" s="64" t="s">
+      <c r="A31" s="58" t="s">
         <v>177</v>
       </c>
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="27" t="s">
         <v>178</v>
       </c>
       <c r="C31" s="26" t="s">
@@ -3144,8 +3153,8 @@
       </c>
     </row>
     <row r="32" spans="1:17">
-      <c r="A32" s="64"/>
-      <c r="B32" s="31" t="s">
+      <c r="A32" s="58"/>
+      <c r="B32" s="28" t="s">
         <v>19</v>
       </c>
       <c r="C32" s="24" t="s">
@@ -3195,8 +3204,8 @@
       </c>
     </row>
     <row r="33" spans="1:17" ht="17" thickBot="1">
-      <c r="A33" s="64"/>
-      <c r="B33" s="32" t="s">
+      <c r="A33" s="58"/>
+      <c r="B33" s="29" t="s">
         <v>67</v>
       </c>
       <c r="C33" s="25" t="s">
@@ -3246,10 +3255,10 @@
       </c>
     </row>
     <row r="34" spans="1:17">
-      <c r="A34" s="64" t="s">
+      <c r="A34" s="58" t="s">
         <v>194</v>
       </c>
-      <c r="B34" s="30" t="s">
+      <c r="B34" s="27" t="s">
         <v>195</v>
       </c>
       <c r="C34" s="26" t="s">
@@ -3299,8 +3308,8 @@
       </c>
     </row>
     <row r="35" spans="1:17">
-      <c r="A35" s="64"/>
-      <c r="B35" s="31" t="s">
+      <c r="A35" s="58"/>
+      <c r="B35" s="28" t="s">
         <v>19</v>
       </c>
       <c r="C35" s="24" t="s">
@@ -3350,8 +3359,8 @@
       </c>
     </row>
     <row r="36" spans="1:17" ht="17" thickBot="1">
-      <c r="A36" s="64"/>
-      <c r="B36" s="32" t="s">
+      <c r="A36" s="58"/>
+      <c r="B36" s="29" t="s">
         <v>67</v>
       </c>
       <c r="C36" s="25" t="s">
@@ -3401,10 +3410,10 @@
       </c>
     </row>
     <row r="37" spans="1:17">
-      <c r="A37" s="64" t="s">
+      <c r="A37" s="58" t="s">
         <v>211</v>
       </c>
-      <c r="B37" s="30" t="s">
+      <c r="B37" s="27" t="s">
         <v>212</v>
       </c>
       <c r="C37" s="26" t="s">
@@ -3454,8 +3463,8 @@
       </c>
     </row>
     <row r="38" spans="1:17">
-      <c r="A38" s="64"/>
-      <c r="B38" s="31" t="s">
+      <c r="A38" s="58"/>
+      <c r="B38" s="28" t="s">
         <v>19</v>
       </c>
       <c r="C38" s="24" t="s">
@@ -3505,8 +3514,8 @@
       </c>
     </row>
     <row r="39" spans="1:17" ht="17" thickBot="1">
-      <c r="A39" s="64"/>
-      <c r="B39" s="32" t="s">
+      <c r="A39" s="58"/>
+      <c r="B39" s="29" t="s">
         <v>67</v>
       </c>
       <c r="C39" s="25" t="s">
@@ -3556,636 +3565,636 @@
       </c>
     </row>
     <row r="40" spans="1:17">
-      <c r="A40" s="62" t="s">
+      <c r="A40" s="56" t="s">
         <v>228</v>
       </c>
-      <c r="B40" s="33" t="s">
+      <c r="B40" s="30" t="s">
         <v>229</v>
       </c>
       <c r="C40" s="12" t="s">
         <v>231</v>
       </c>
-      <c r="D40" s="36" t="s">
+      <c r="D40" s="33" t="s">
         <v>232</v>
       </c>
-      <c r="E40" s="36" t="s">
+      <c r="E40" s="33" t="s">
         <v>233</v>
       </c>
-      <c r="F40" s="36" t="s">
+      <c r="F40" s="33" t="s">
         <v>234</v>
       </c>
       <c r="G40" s="12" t="s">
         <v>236</v>
       </c>
-      <c r="H40" s="46" t="s">
+      <c r="H40" s="40" t="s">
         <v>238</v>
       </c>
-      <c r="I40" s="36" t="s">
+      <c r="I40" s="33" t="s">
         <v>239</v>
       </c>
-      <c r="J40" s="36" t="s">
+      <c r="J40" s="33" t="s">
         <v>240</v>
       </c>
-      <c r="K40" s="36" t="s">
+      <c r="K40" s="33" t="s">
         <v>241</v>
       </c>
-      <c r="L40" s="36" t="s">
+      <c r="L40" s="33" t="s">
         <v>242</v>
       </c>
-      <c r="M40" s="42" t="s">
+      <c r="M40" s="36" t="s">
         <v>243</v>
       </c>
-      <c r="N40" s="36" t="s">
+      <c r="N40" s="33" t="s">
         <v>244</v>
       </c>
-      <c r="O40" s="36" t="s">
+      <c r="O40" s="33" t="s">
         <v>245</v>
       </c>
-      <c r="P40" s="46" t="s">
+      <c r="P40" s="40" t="s">
         <v>247</v>
       </c>
-      <c r="Q40" s="36" t="s">
+      <c r="Q40" s="33" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="41" spans="1:17">
-      <c r="A41" s="62"/>
-      <c r="B41" s="34" t="s">
+      <c r="A41" s="56"/>
+      <c r="B41" s="31" t="s">
         <v>230</v>
       </c>
       <c r="C41" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D41" s="37" t="s">
+      <c r="D41" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="E41" s="37" t="s">
+      <c r="E41" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="F41" s="37" t="s">
+      <c r="F41" s="34" t="s">
         <v>235</v>
       </c>
       <c r="G41" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="H41" s="50" t="s">
+      <c r="H41" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="I41" s="37" t="s">
+      <c r="I41" s="34" t="s">
         <v>237</v>
       </c>
-      <c r="J41" s="37" t="s">
+      <c r="J41" s="34" t="s">
         <v>230</v>
       </c>
-      <c r="K41" s="37" t="s">
+      <c r="K41" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="L41" s="37" t="s">
+      <c r="L41" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="M41" s="43" t="s">
+      <c r="M41" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="N41" s="37" t="s">
+      <c r="N41" s="34" t="s">
         <v>235</v>
       </c>
-      <c r="O41" s="37" t="s">
+      <c r="O41" s="34" t="s">
         <v>246</v>
       </c>
-      <c r="P41" s="50" t="s">
+      <c r="P41" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="Q41" s="37" t="s">
+      <c r="Q41" s="34" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="42" spans="1:17" ht="17" thickBot="1">
-      <c r="A42" s="62"/>
-      <c r="B42" s="35" t="s">
+      <c r="A42" s="56"/>
+      <c r="B42" s="32" t="s">
         <v>20</v>
       </c>
       <c r="C42" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D42" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="E42" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="F42" s="38" t="s">
+      <c r="D42" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="E42" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="F42" s="35" t="s">
         <v>20</v>
       </c>
       <c r="G42" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="H42" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="I42" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="J42" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="K42" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="L42" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="M42" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="N42" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="O42" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="P42" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q42" s="38" t="s">
+      <c r="H42" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="I42" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="J42" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="K42" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="L42" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="M42" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="N42" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="O42" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="P42" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q42" s="35" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:17">
-      <c r="A43" s="62" t="s">
+      <c r="A43" s="56" t="s">
         <v>249</v>
       </c>
-      <c r="B43" s="33" t="s">
+      <c r="B43" s="30" t="s">
         <v>250</v>
       </c>
       <c r="C43" s="12" t="s">
         <v>251</v>
       </c>
-      <c r="D43" s="36" t="s">
+      <c r="D43" s="33" t="s">
         <v>252</v>
       </c>
-      <c r="E43" s="39" t="s">
+      <c r="E43" s="60" t="s">
         <v>253</v>
       </c>
-      <c r="F43" s="36" t="s">
+      <c r="F43" s="33" t="s">
         <v>254</v>
       </c>
       <c r="G43" s="12" t="s">
         <v>255</v>
       </c>
-      <c r="H43" s="46" t="s">
+      <c r="H43" s="40" t="s">
         <v>256</v>
       </c>
-      <c r="I43" s="36" t="s">
+      <c r="I43" s="33" t="s">
         <v>257</v>
       </c>
-      <c r="J43" s="36" t="s">
+      <c r="J43" s="33" t="s">
         <v>258</v>
       </c>
-      <c r="K43" s="42" t="s">
+      <c r="K43" s="36" t="s">
         <v>259</v>
       </c>
-      <c r="L43" s="36" t="s">
+      <c r="L43" s="33" t="s">
         <v>260</v>
       </c>
-      <c r="M43" s="39" t="s">
+      <c r="M43" s="60" t="s">
         <v>261</v>
       </c>
-      <c r="N43" s="36" t="s">
+      <c r="N43" s="33" t="s">
         <v>262</v>
       </c>
-      <c r="O43" s="36" t="s">
+      <c r="O43" s="33" t="s">
         <v>263</v>
       </c>
-      <c r="P43" s="46" t="s">
+      <c r="P43" s="40" t="s">
         <v>264</v>
       </c>
-      <c r="Q43" s="36" t="s">
+      <c r="Q43" s="33" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="44" spans="1:17">
-      <c r="A44" s="62"/>
-      <c r="B44" s="34" t="s">
+      <c r="A44" s="56"/>
+      <c r="B44" s="31" t="s">
         <v>230</v>
       </c>
       <c r="C44" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D44" s="37" t="s">
+      <c r="D44" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="E44" s="40" t="s">
+      <c r="E44" s="61" t="s">
         <v>83</v>
       </c>
-      <c r="F44" s="37" t="s">
+      <c r="F44" s="34" t="s">
         <v>235</v>
       </c>
       <c r="G44" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="H44" s="50" t="s">
+      <c r="H44" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="I44" s="37" t="s">
+      <c r="I44" s="34" t="s">
         <v>237</v>
       </c>
-      <c r="J44" s="37" t="s">
+      <c r="J44" s="34" t="s">
         <v>230</v>
       </c>
-      <c r="K44" s="43" t="s">
+      <c r="K44" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="L44" s="37" t="s">
+      <c r="L44" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="M44" s="40" t="s">
+      <c r="M44" s="61" t="s">
         <v>83</v>
       </c>
-      <c r="N44" s="37" t="s">
+      <c r="N44" s="34" t="s">
         <v>235</v>
       </c>
-      <c r="O44" s="37" t="s">
+      <c r="O44" s="34" t="s">
         <v>246</v>
       </c>
-      <c r="P44" s="50" t="s">
+      <c r="P44" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="Q44" s="37" t="s">
+      <c r="Q44" s="34" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="45" spans="1:17" ht="17" thickBot="1">
-      <c r="A45" s="62"/>
-      <c r="B45" s="35" t="s">
+      <c r="A45" s="56"/>
+      <c r="B45" s="32" t="s">
         <v>20</v>
       </c>
       <c r="C45" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D45" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="E45" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="F45" s="38" t="s">
+      <c r="D45" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="E45" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="F45" s="35" t="s">
         <v>20</v>
       </c>
       <c r="G45" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="H45" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="I45" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="J45" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="K45" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="L45" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="M45" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="N45" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="O45" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="P45" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q45" s="38" t="s">
+      <c r="H45" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="I45" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="J45" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="K45" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="L45" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="M45" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="N45" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="O45" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="P45" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q45" s="35" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:17">
-      <c r="A46" s="62" t="s">
+      <c r="A46" s="56" t="s">
         <v>266</v>
       </c>
-      <c r="B46" s="33" t="s">
+      <c r="B46" s="30" t="s">
         <v>267</v>
       </c>
       <c r="C46" s="12" t="s">
         <v>268</v>
       </c>
-      <c r="D46" s="36" t="s">
+      <c r="D46" s="33" t="s">
         <v>269</v>
       </c>
-      <c r="E46" s="27" t="s">
+      <c r="E46" s="63" t="s">
         <v>270</v>
       </c>
-      <c r="F46" s="36" t="s">
+      <c r="F46" s="33" t="s">
         <v>272</v>
       </c>
       <c r="G46" s="12" t="s">
         <v>273</v>
       </c>
-      <c r="H46" s="46" t="s">
+      <c r="H46" s="40" t="s">
         <v>274</v>
       </c>
-      <c r="I46" s="36" t="s">
+      <c r="I46" s="33" t="s">
         <v>275</v>
       </c>
-      <c r="J46" s="36" t="s">
+      <c r="J46" s="33" t="s">
         <v>276</v>
       </c>
-      <c r="K46" s="42" t="s">
+      <c r="K46" s="66" t="s">
         <v>277</v>
       </c>
-      <c r="L46" s="36" t="s">
+      <c r="L46" s="33" t="s">
         <v>278</v>
       </c>
-      <c r="M46" s="27" t="s">
+      <c r="M46" s="63" t="s">
         <v>279</v>
       </c>
-      <c r="N46" s="36" t="s">
+      <c r="N46" s="33" t="s">
         <v>280</v>
       </c>
-      <c r="O46" s="36" t="s">
+      <c r="O46" s="33" t="s">
         <v>263</v>
       </c>
-      <c r="P46" s="46" t="s">
+      <c r="P46" s="40" t="s">
         <v>281</v>
       </c>
-      <c r="Q46" s="36" t="s">
+      <c r="Q46" s="33" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="47" spans="1:17">
-      <c r="A47" s="62"/>
-      <c r="B47" s="34" t="s">
+      <c r="A47" s="56"/>
+      <c r="B47" s="31" t="s">
         <v>230</v>
       </c>
       <c r="C47" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D47" s="37" t="s">
+      <c r="D47" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="E47" s="28" t="s">
+      <c r="E47" s="64" t="s">
         <v>271</v>
       </c>
-      <c r="F47" s="37" t="s">
+      <c r="F47" s="34" t="s">
         <v>235</v>
       </c>
       <c r="G47" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="H47" s="50" t="s">
+      <c r="H47" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="I47" s="37" t="s">
+      <c r="I47" s="34" t="s">
         <v>237</v>
       </c>
-      <c r="J47" s="37" t="s">
+      <c r="J47" s="34" t="s">
         <v>230</v>
       </c>
-      <c r="K47" s="43" t="s">
-        <v>26</v>
-      </c>
-      <c r="L47" s="37" t="s">
+      <c r="K47" s="67" t="s">
+        <v>26</v>
+      </c>
+      <c r="L47" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="M47" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="N47" s="37" t="s">
+      <c r="M47" s="64" t="s">
+        <v>26</v>
+      </c>
+      <c r="N47" s="34" t="s">
         <v>235</v>
       </c>
-      <c r="O47" s="37" t="s">
+      <c r="O47" s="34" t="s">
         <v>246</v>
       </c>
-      <c r="P47" s="50" t="s">
+      <c r="P47" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="Q47" s="37" t="s">
+      <c r="Q47" s="34" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="48" spans="1:17" ht="17" thickBot="1">
-      <c r="A48" s="62"/>
-      <c r="B48" s="35" t="s">
+      <c r="A48" s="56"/>
+      <c r="B48" s="32" t="s">
         <v>20</v>
       </c>
       <c r="C48" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D48" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="E48" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="F48" s="38" t="s">
+      <c r="D48" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="E48" s="65" t="s">
+        <v>20</v>
+      </c>
+      <c r="F48" s="35" t="s">
         <v>20</v>
       </c>
       <c r="G48" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="H48" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="I48" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="J48" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="K48" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="L48" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="M48" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="N48" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="O48" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="P48" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q48" s="38" t="s">
+      <c r="H48" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="I48" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="J48" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="K48" s="68" t="s">
+        <v>20</v>
+      </c>
+      <c r="L48" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="M48" s="65" t="s">
+        <v>20</v>
+      </c>
+      <c r="N48" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="O48" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="P48" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q48" s="35" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="49" spans="1:17">
-      <c r="A49" s="62" t="s">
+      <c r="A49" s="56" t="s">
         <v>283</v>
       </c>
-      <c r="B49" s="33" t="s">
+      <c r="B49" s="30" t="s">
         <v>284</v>
       </c>
       <c r="C49" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="D49" s="36" t="s">
+      <c r="D49" s="33" t="s">
         <v>286</v>
       </c>
-      <c r="E49" s="39" t="s">
+      <c r="E49" s="60" t="s">
         <v>287</v>
       </c>
-      <c r="F49" s="36" t="s">
+      <c r="F49" s="33" t="s">
         <v>288</v>
       </c>
       <c r="G49" s="12" t="s">
         <v>289</v>
       </c>
-      <c r="H49" s="46" t="s">
+      <c r="H49" s="40" t="s">
         <v>290</v>
       </c>
-      <c r="I49" s="36" t="s">
+      <c r="I49" s="33" t="s">
         <v>291</v>
       </c>
-      <c r="J49" s="36" t="s">
+      <c r="J49" s="33" t="s">
         <v>292</v>
       </c>
-      <c r="K49" s="27" t="s">
+      <c r="K49" s="63" t="s">
         <v>293</v>
       </c>
-      <c r="L49" s="36" t="s">
+      <c r="L49" s="33" t="s">
         <v>294</v>
       </c>
-      <c r="M49" s="39" t="s">
+      <c r="M49" s="60" t="s">
         <v>295</v>
       </c>
-      <c r="N49" s="36" t="s">
+      <c r="N49" s="33" t="s">
         <v>296</v>
       </c>
-      <c r="O49" s="36" t="s">
+      <c r="O49" s="33" t="s">
         <v>263</v>
       </c>
-      <c r="P49" s="46" t="s">
+      <c r="P49" s="40" t="s">
         <v>297</v>
       </c>
-      <c r="Q49" s="36" t="s">
+      <c r="Q49" s="33" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="50" spans="1:17">
-      <c r="A50" s="62"/>
-      <c r="B50" s="34" t="s">
+      <c r="A50" s="56"/>
+      <c r="B50" s="31" t="s">
         <v>230</v>
       </c>
       <c r="C50" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D50" s="37" t="s">
+      <c r="D50" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="E50" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="F50" s="37" t="s">
+      <c r="E50" s="61" t="s">
+        <v>19</v>
+      </c>
+      <c r="F50" s="34" t="s">
         <v>235</v>
       </c>
       <c r="G50" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="H50" s="50" t="s">
+      <c r="H50" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="I50" s="37" t="s">
+      <c r="I50" s="34" t="s">
         <v>237</v>
       </c>
-      <c r="J50" s="37" t="s">
+      <c r="J50" s="34" t="s">
         <v>230</v>
       </c>
-      <c r="K50" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="L50" s="37" t="s">
+      <c r="K50" s="64" t="s">
+        <v>26</v>
+      </c>
+      <c r="L50" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="M50" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="N50" s="37" t="s">
+      <c r="M50" s="61" t="s">
+        <v>19</v>
+      </c>
+      <c r="N50" s="34" t="s">
         <v>235</v>
       </c>
-      <c r="O50" s="37" t="s">
+      <c r="O50" s="34" t="s">
         <v>246</v>
       </c>
-      <c r="P50" s="50" t="s">
+      <c r="P50" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="Q50" s="37" t="s">
+      <c r="Q50" s="34" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="51" spans="1:17" ht="17" thickBot="1">
-      <c r="A51" s="63"/>
-      <c r="B51" s="35" t="s">
+      <c r="A51" s="59"/>
+      <c r="B51" s="32" t="s">
         <v>20</v>
       </c>
       <c r="C51" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="D51" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="E51" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="F51" s="38" t="s">
+      <c r="D51" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="E51" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="F51" s="35" t="s">
         <v>20</v>
       </c>
       <c r="G51" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="H51" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="I51" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="J51" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="K51" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="L51" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="M51" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="N51" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="O51" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="P51" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q51" s="38" t="s">
+      <c r="H51" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="I51" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="J51" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="K51" s="65" t="s">
+        <v>20</v>
+      </c>
+      <c r="L51" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="M51" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="N51" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="O51" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="P51" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q51" s="35" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="52" spans="1:17" ht="17" thickBot="1">
-      <c r="B52" s="60" t="s">
+      <c r="B52" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C52" s="61" t="s">
+      <c r="C52" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="D52" s="61" t="s">
+      <c r="D52" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="E52" s="61" t="s">
+      <c r="E52" s="55" t="s">
         <v>4</v>
       </c>
       <c r="F52" s="4" t="s">
@@ -4200,16 +4209,16 @@
       <c r="I52" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J52" s="61" t="s">
+      <c r="J52" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="K52" s="61" t="s">
+      <c r="K52" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="L52" s="61" t="s">
+      <c r="L52" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="M52" s="61" t="s">
+      <c r="M52" s="55" t="s">
         <v>12</v>
       </c>
       <c r="N52" s="4" t="s">
@@ -4226,16 +4235,16 @@
       </c>
     </row>
     <row r="53" spans="1:17" ht="17" thickBot="1">
-      <c r="J53" s="60" t="s">
+      <c r="J53" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="K53" s="61" t="s">
+      <c r="K53" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="L53" s="61" t="s">
+      <c r="L53" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="M53" s="61" t="s">
+      <c r="M53" s="55" t="s">
         <v>4</v>
       </c>
       <c r="N53" s="4" t="s">
@@ -4253,12 +4262,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="A16:A18"/>
     <mergeCell ref="A40:A42"/>
     <mergeCell ref="A43:A45"/>
     <mergeCell ref="A46:A48"/>
@@ -4269,6 +4272,12 @@
     <mergeCell ref="A31:A33"/>
     <mergeCell ref="A34:A36"/>
     <mergeCell ref="A37:A39"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A16:A18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>